<commit_message>
feat: Excluir arquivo apos importar dados
</commit_message>
<xml_diff>
--- a/tests/assets/operacoes-teste.xlsx
+++ b/tests/assets/operacoes-teste.xlsx
@@ -566,7 +566,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -582,7 +582,7 @@
     <col min="14" max="14" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="12.75">
       <c r="A1" s="34" t="s">
         <v>21</v>
       </c>
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" ht="12.75">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -866,7 +866,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" ht="12.75">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
@@ -880,7 +880,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" ht="12.75">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
@@ -895,7 +895,7 @@
       <c r="M9" s="7"/>
       <c r="N9" s="16"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" ht="12.75">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -909,7 +909,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" ht="12.75">
       <c r="B11" s="20"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -923,7 +923,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" ht="12.75">
       <c r="B12" s="20"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -937,7 +937,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" ht="12.75">
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -951,7 +951,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" ht="12.75">
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -965,7 +965,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" ht="12.75">
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -980,7 +980,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="16"/>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" ht="12.75">
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -995,7 +995,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" ht="12.75">
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -1010,7 +1010,7 @@
       <c r="M17" s="7"/>
       <c r="N17" s="16"/>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" ht="12.75">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="14"/>
@@ -1024,7 +1024,7 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" ht="12.75">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1038,7 +1038,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" ht="12.75">
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1052,7 +1052,7 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" ht="12.75">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1067,7 +1067,7 @@
       <c r="M21" s="7"/>
       <c r="N21" s="16"/>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:14" ht="12.75">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1081,7 +1081,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:14" ht="12.75">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -1096,7 +1096,7 @@
       <c r="M23" s="7"/>
       <c r="N23" s="16"/>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:14" ht="12.75">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -1110,7 +1110,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:14" ht="12.75">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -1124,7 +1124,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" ht="12.75">
       <c r="B26" s="9"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1139,7 +1139,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="16"/>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" ht="12.75">
       <c r="B27" s="9"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -1153,7 +1153,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" ht="12.75">
       <c r="B28" s="9"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -1168,7 +1168,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="16"/>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" ht="12.75">
       <c r="B29" s="9"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -1183,7 +1183,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="16"/>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" ht="12.75">
       <c r="B30" s="9"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
@@ -1198,7 +1198,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="16"/>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" ht="12.75">
       <c r="B31" s="9"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
@@ -1212,7 +1212,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" ht="12.75">
       <c r="B32" s="9"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -1227,7 +1227,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="16"/>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" ht="12.75">
       <c r="B33" s="9"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -1242,7 +1242,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="16"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" ht="12.75">
       <c r="B34" s="9"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -1257,7 +1257,7 @@
       <c r="M34" s="7"/>
       <c r="N34" s="16"/>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" ht="12.75">
       <c r="B35" s="9"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -1272,7 +1272,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="16"/>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:14" ht="12.75">
       <c r="B36" s="9"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
@@ -1287,7 +1287,7 @@
       <c r="M36" s="7"/>
       <c r="N36" s="16"/>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:14" ht="12.75">
       <c r="B37" s="23"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
@@ -1302,7 +1302,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="16"/>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="2:14" ht="12.75">
       <c r="B38" s="23"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -1317,7 +1317,7 @@
       <c r="M38" s="7"/>
       <c r="N38" s="18"/>
     </row>
-    <row r="39" spans="2:14">
+    <row r="39" spans="2:14" ht="12.75">
       <c r="B39" s="23"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
@@ -1331,7 +1331,7 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="2:14">
+    <row r="40" spans="2:14" ht="12.75">
       <c r="B40" s="17"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
@@ -1346,7 +1346,7 @@
       <c r="M40" s="7"/>
       <c r="N40" s="16"/>
     </row>
-    <row r="41" spans="2:14">
+    <row r="41" spans="2:14" ht="12.75">
       <c r="B41" s="17"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -1361,7 +1361,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="16"/>
     </row>
-    <row r="42" spans="2:14">
+    <row r="42" spans="2:14" ht="12.75">
       <c r="B42" s="17"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
@@ -1375,7 +1375,7 @@
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
     </row>
-    <row r="43" spans="2:14">
+    <row r="43" spans="2:14" ht="12.75">
       <c r="B43" s="17"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
@@ -1390,7 +1390,7 @@
       <c r="M43" s="7"/>
       <c r="N43" s="16"/>
     </row>
-    <row r="44" spans="2:14">
+    <row r="44" spans="2:14" ht="12.75">
       <c r="B44" s="17"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
@@ -1405,7 +1405,7 @@
       <c r="M44" s="7"/>
       <c r="N44" s="16"/>
     </row>
-    <row r="45" spans="2:14">
+    <row r="45" spans="2:14" ht="12.75">
       <c r="B45" s="17"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
@@ -1420,7 +1420,7 @@
       <c r="M45" s="7"/>
       <c r="N45" s="16"/>
     </row>
-    <row r="46" spans="2:14">
+    <row r="46" spans="2:14" ht="12.75">
       <c r="B46" s="17"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -1435,7 +1435,7 @@
       <c r="M46" s="7"/>
       <c r="N46" s="18"/>
     </row>
-    <row r="47" spans="2:14">
+    <row r="47" spans="2:14" ht="12.75">
       <c r="B47" s="17"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
@@ -1450,7 +1450,7 @@
       <c r="M47" s="7"/>
       <c r="N47" s="16"/>
     </row>
-    <row r="48" spans="2:14">
+    <row r="48" spans="2:14" ht="12.75">
       <c r="B48" s="17"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
@@ -1465,7 +1465,7 @@
       <c r="M48" s="7"/>
       <c r="N48" s="16"/>
     </row>
-    <row r="49" spans="2:14">
+    <row r="49" spans="2:14" ht="12.75">
       <c r="B49" s="17"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
@@ -1480,7 +1480,7 @@
       <c r="M49" s="7"/>
       <c r="N49" s="16"/>
     </row>
-    <row r="50" spans="2:14">
+    <row r="50" spans="2:14" ht="12.75">
       <c r="B50" s="17"/>
       <c r="C50" s="22"/>
       <c r="D50" s="6"/>
@@ -1495,7 +1495,7 @@
       <c r="M50" s="7"/>
       <c r="N50" s="16"/>
     </row>
-    <row r="51" spans="2:14">
+    <row r="51" spans="2:14" ht="12.75">
       <c r="B51" s="17"/>
       <c r="C51" s="22"/>
       <c r="D51" s="6"/>
@@ -1510,7 +1510,7 @@
       <c r="M51" s="7"/>
       <c r="N51" s="16"/>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="2:14" ht="12.75">
       <c r="B52" s="17"/>
       <c r="C52" s="22"/>
       <c r="D52" s="6"/>
@@ -1524,7 +1524,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="2:14" ht="12.75">
       <c r="B53" s="17"/>
       <c r="C53" s="22"/>
       <c r="D53" s="6"/>
@@ -1539,7 +1539,7 @@
       <c r="M53" s="7"/>
       <c r="N53" s="16"/>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="2:14" ht="12.75">
       <c r="B54" s="17"/>
       <c r="C54" s="22"/>
       <c r="D54" s="6"/>
@@ -1554,7 +1554,7 @@
       <c r="M54" s="7"/>
       <c r="N54" s="18"/>
     </row>
-    <row r="55" spans="2:14">
+    <row r="55" spans="2:14" ht="12.75">
       <c r="B55" s="17"/>
       <c r="C55" s="22"/>
       <c r="D55" s="6"/>
@@ -1569,7 +1569,7 @@
       <c r="M55" s="7"/>
       <c r="N55" s="16"/>
     </row>
-    <row r="56" spans="2:14">
+    <row r="56" spans="2:14" ht="12.75">
       <c r="B56" s="17"/>
       <c r="C56" s="22"/>
       <c r="D56" s="6"/>
@@ -1584,7 +1584,7 @@
       <c r="M56" s="7"/>
       <c r="N56" s="16"/>
     </row>
-    <row r="57" spans="2:14">
+    <row r="57" spans="2:14" ht="12.75">
       <c r="B57" s="17"/>
       <c r="C57" s="22"/>
       <c r="D57" s="6"/>
@@ -1599,7 +1599,7 @@
       <c r="M57" s="7"/>
       <c r="N57" s="16"/>
     </row>
-    <row r="58" spans="2:14">
+    <row r="58" spans="2:14" ht="12.75">
       <c r="B58" s="17"/>
       <c r="C58" s="22"/>
       <c r="D58" s="6"/>
@@ -1614,7 +1614,7 @@
       <c r="M58" s="7"/>
       <c r="N58" s="16"/>
     </row>
-    <row r="59" spans="2:14">
+    <row r="59" spans="2:14" ht="12.75">
       <c r="B59" s="17"/>
       <c r="C59" s="22"/>
       <c r="D59" s="6"/>
@@ -1629,7 +1629,7 @@
       <c r="M59" s="7"/>
       <c r="N59" s="16"/>
     </row>
-    <row r="60" spans="2:14">
+    <row r="60" spans="2:14" ht="12.75">
       <c r="B60" s="20"/>
       <c r="C60" s="21"/>
       <c r="D60" s="21"/>
@@ -1644,7 +1644,7 @@
       <c r="M60" s="7"/>
       <c r="N60" s="16"/>
     </row>
-    <row r="61" spans="2:14">
+    <row r="61" spans="2:14" ht="12.75">
       <c r="B61" s="20"/>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
@@ -1659,7 +1659,7 @@
       <c r="M61" s="7"/>
       <c r="N61" s="16"/>
     </row>
-    <row r="62" spans="2:14">
+    <row r="62" spans="2:14" ht="12.75">
       <c r="B62" s="20"/>
       <c r="C62" s="21"/>
       <c r="D62" s="21"/>
@@ -1674,7 +1674,7 @@
       <c r="M62" s="7"/>
       <c r="N62" s="16"/>
     </row>
-    <row r="63" spans="2:14">
+    <row r="63" spans="2:14" ht="12.75">
       <c r="B63" s="17"/>
       <c r="C63" s="22"/>
       <c r="D63" s="6"/>
@@ -1689,7 +1689,7 @@
       <c r="M63" s="7"/>
       <c r="N63" s="16"/>
     </row>
-    <row r="64" spans="2:14">
+    <row r="64" spans="2:14" ht="12.75">
       <c r="B64" s="17"/>
       <c r="C64" s="22"/>
       <c r="D64" s="6"/>
@@ -1704,7 +1704,7 @@
       <c r="M64" s="7"/>
       <c r="N64" s="18"/>
     </row>
-    <row r="65" spans="2:14">
+    <row r="65" spans="2:14" ht="12.75">
       <c r="B65" s="17"/>
       <c r="C65" s="22"/>
       <c r="D65" s="6"/>
@@ -1719,7 +1719,7 @@
       <c r="M65" s="7"/>
       <c r="N65" s="16"/>
     </row>
-    <row r="66" spans="2:14">
+    <row r="66" spans="2:14" ht="12.75">
       <c r="B66" s="17"/>
       <c r="C66" s="22"/>
       <c r="D66" s="6"/>
@@ -1734,7 +1734,7 @@
       <c r="M66" s="7"/>
       <c r="N66" s="16"/>
     </row>
-    <row r="67" spans="2:14">
+    <row r="67" spans="2:14" ht="12.75">
       <c r="B67" s="17"/>
       <c r="C67" s="22"/>
       <c r="D67" s="6"/>
@@ -1749,7 +1749,7 @@
       <c r="M67" s="7"/>
       <c r="N67" s="16"/>
     </row>
-    <row r="68" spans="2:14">
+    <row r="68" spans="2:14" ht="12.75">
       <c r="B68" s="17"/>
       <c r="C68" s="22"/>
       <c r="D68" s="6"/>
@@ -1764,7 +1764,7 @@
       <c r="M68" s="7"/>
       <c r="N68" s="16"/>
     </row>
-    <row r="69" spans="2:14">
+    <row r="69" spans="2:14" ht="12.75">
       <c r="B69" s="17"/>
       <c r="C69" s="22"/>
       <c r="D69" s="6"/>
@@ -1779,7 +1779,7 @@
       <c r="M69" s="7"/>
       <c r="N69" s="16"/>
     </row>
-    <row r="70" spans="2:14">
+    <row r="70" spans="2:14" ht="12.75">
       <c r="B70" s="17"/>
       <c r="C70" s="22"/>
       <c r="D70" s="6"/>
@@ -1794,7 +1794,7 @@
       <c r="M70" s="7"/>
       <c r="N70" s="16"/>
     </row>
-    <row r="71" spans="2:14">
+    <row r="71" spans="2:14" ht="12.75">
       <c r="B71" s="17"/>
       <c r="C71" s="22"/>
       <c r="D71" s="6"/>
@@ -1809,7 +1809,7 @@
       <c r="M71" s="7"/>
       <c r="N71" s="16"/>
     </row>
-    <row r="72" spans="2:14">
+    <row r="72" spans="2:14" ht="12.75">
       <c r="B72" s="17"/>
       <c r="C72" s="22"/>
       <c r="D72" s="6"/>
@@ -1824,7 +1824,7 @@
       <c r="M72" s="7"/>
       <c r="N72" s="16"/>
     </row>
-    <row r="73" spans="2:14">
+    <row r="73" spans="2:14" ht="12.75">
       <c r="B73" s="17"/>
       <c r="C73" s="22"/>
       <c r="D73" s="6"/>
@@ -1839,7 +1839,7 @@
       <c r="M73" s="7"/>
       <c r="N73" s="16"/>
     </row>
-    <row r="74" spans="2:14">
+    <row r="74" spans="2:14" ht="12.75">
       <c r="B74" s="17"/>
       <c r="C74" s="22"/>
       <c r="D74" s="6"/>
@@ -1854,7 +1854,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="16"/>
     </row>
-    <row r="75" spans="2:14">
+    <row r="75" spans="2:14" ht="12.75">
       <c r="B75" s="17"/>
       <c r="C75" s="22"/>
       <c r="D75" s="6"/>
@@ -1869,7 +1869,7 @@
       <c r="M75" s="7"/>
       <c r="N75" s="16"/>
     </row>
-    <row r="76" spans="2:14">
+    <row r="76" spans="2:14" ht="12.75">
       <c r="B76" s="17"/>
       <c r="C76" s="22"/>
       <c r="D76" s="6"/>
@@ -1884,7 +1884,7 @@
       <c r="M76" s="7"/>
       <c r="N76" s="16"/>
     </row>
-    <row r="77" spans="2:14">
+    <row r="77" spans="2:14" ht="12.75">
       <c r="B77" s="17"/>
       <c r="C77" s="22"/>
       <c r="D77" s="6"/>
@@ -1899,7 +1899,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="16"/>
     </row>
-    <row r="78" spans="2:14">
+    <row r="78" spans="2:14" ht="12.75">
       <c r="B78" s="17"/>
       <c r="C78" s="22"/>
       <c r="D78" s="6"/>
@@ -1914,7 +1914,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="16"/>
     </row>
-    <row r="79" spans="2:14">
+    <row r="79" spans="2:14" ht="12.75">
       <c r="B79" s="17"/>
       <c r="C79" s="22"/>
       <c r="D79" s="6"/>
@@ -1929,7 +1929,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="16"/>
     </row>
-    <row r="80" spans="2:14">
+    <row r="80" spans="2:14" ht="12.75">
       <c r="B80" s="17"/>
       <c r="C80" s="5"/>
       <c r="D80" s="3"/>
@@ -1944,7 +1944,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="16"/>
     </row>
-    <row r="81" spans="2:14">
+    <row r="81" spans="2:14" ht="12.75">
       <c r="B81" s="17"/>
       <c r="C81" s="5"/>
       <c r="D81" s="3"/>
@@ -1959,7 +1959,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="16"/>
     </row>
-    <row r="82" spans="2:14">
+    <row r="82" spans="2:14" ht="12.75">
       <c r="B82" s="17"/>
       <c r="C82" s="5"/>
       <c r="D82" s="3"/>
@@ -1974,7 +1974,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="16"/>
     </row>
-    <row r="83" spans="2:14">
+    <row r="83" spans="2:14" ht="12.75">
       <c r="B83" s="17"/>
       <c r="C83" s="5"/>
       <c r="D83" s="3"/>
@@ -1989,7 +1989,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="16"/>
     </row>
-    <row r="84" spans="2:14">
+    <row r="84" spans="2:14" ht="12.75">
       <c r="B84" s="17"/>
       <c r="C84" s="5"/>
       <c r="D84" s="3"/>
@@ -2004,7 +2004,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="16"/>
     </row>
-    <row r="85" spans="2:14">
+    <row r="85" spans="2:14" ht="12.75">
       <c r="B85" s="17"/>
       <c r="C85" s="5"/>
       <c r="D85" s="3"/>
@@ -2019,7 +2019,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="16"/>
     </row>
-    <row r="86" spans="2:14">
+    <row r="86" spans="2:14" ht="12.75">
       <c r="B86" s="17"/>
       <c r="C86" s="5"/>
       <c r="D86" s="3"/>
@@ -2034,7 +2034,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="16"/>
     </row>
-    <row r="87" spans="2:14">
+    <row r="87" spans="2:14" ht="12.75">
       <c r="B87" s="17"/>
       <c r="C87" s="5"/>
       <c r="D87" s="3"/>
@@ -2049,7 +2049,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="16"/>
     </row>
-    <row r="88" spans="2:14">
+    <row r="88" spans="2:14" ht="12.75">
       <c r="B88" s="17"/>
       <c r="C88" s="5"/>
       <c r="D88" s="3"/>
@@ -2064,7 +2064,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="16"/>
     </row>
-    <row r="89" spans="2:14">
+    <row r="89" spans="2:14" ht="12.75">
       <c r="B89" s="17"/>
       <c r="C89" s="5"/>
       <c r="D89" s="3"/>
@@ -2079,7 +2079,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="16"/>
     </row>
-    <row r="90" spans="2:14">
+    <row r="90" spans="2:14" ht="12.75">
       <c r="B90" s="17"/>
       <c r="C90" s="5"/>
       <c r="D90" s="3"/>
@@ -2094,7 +2094,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="16"/>
     </row>
-    <row r="91" spans="2:14">
+    <row r="91" spans="2:14" ht="12.75">
       <c r="B91" s="17"/>
       <c r="C91" s="5"/>
       <c r="D91" s="3"/>

</xml_diff>